<commit_message>
Made excel templates have correct fields
</commit_message>
<xml_diff>
--- a/Cards/ActionData/Action-Front.xlsx
+++ b/Cards/ActionData/Action-Front.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Github Repos\TEAM-TEAM-TraitorCards\Cards\ActionData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5DB92AC-73B6-4812-BA8E-08A4986F9037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E6318E-A03A-4A43-BC53-15FB37E7DF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E0E38A4-A720-4B05-94AE-F55473173966}"/>
   </bookViews>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>@Image</t>
+  </si>
+  <si>
+    <t>Effect</t>
   </si>
 </sst>
 </file>
@@ -91,12 +94,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -436,17 +442,17 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="82.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -456,10 +462,12 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>